<commit_message>
applied a patch for tabs having 0 records and tabs having more than 10 records
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
+++ b/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BD2BD5-389C-4953-84BF-1C51ED83BDBB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD925796-E5D1-4A5C-B8F7-D543CBC40804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>WebExcel</t>
   </si>
@@ -43,20 +43,85 @@
     <t>dbExcel</t>
   </si>
   <si>
-    <t xml:space="preserve">MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN ['Akita'] WITH DISTINCT c AS c, p, s, demo, diag RETURN coalesce(c.case_id,'') AS `Case ID` , coalesce(s.clinical_study_designation,'') AS `Study Code` , coalesce(s.clinical_study_type,'') AS  `Study Type`, coalesce(demo.breed,'') AS Breed , coalesce(diag.disease_term,'') AS Diagnosis , coalesce(diag.stage_of_disease,'') AS `Stage of Disease` ,  coalesce(demo.patient_age_at_enrollment,'') AS Age , coalesce(demo.sex,'') AS Sex , coalesce(demo.neutered_indicator,'') AS  `Neutered Status`
+    <t>TC01_Canine_Filter_Breed-Akita_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC01_Canine_Filter_Breed-Akita_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN['Akita']  OPTIONAL MATCH (f:file)-[*]-&gt;(c), (samp:sample)-[*]-&gt;(c) WITH DISTINCT c AS c, p, s, demo, diag, f, samp RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(samp)) as number_of_sample , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
+  </si>
+  <si>
+    <t>StatQuery</t>
+  </si>
+  <si>
+    <t>TabName</t>
+  </si>
+  <si>
+    <t>CasesTab</t>
+  </si>
+  <si>
+    <t>SamplesTab</t>
+  </si>
+  <si>
+    <t>FilesTab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE demo.breed IN ['Akita']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co
+RETURN  coalesce(c.case_id, '') AS `Case ID` ,
+        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
+        coalesce(s.clinical_study_type, '') AS  `Study Type`,
+        coalesce(demo.breed, '') AS Breed ,
+        coalesce(diag.disease_term, '') AS Diagnosis ,
+        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
+        coalesce(demo.patient_age_at_enrollment, '') AS Age ,
+        coalesce(demo.sex, '') AS Sex ,
+        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+        coalesce(demo.weight, '') AS `Weight (kg)`,
+        coalesce(diag.best_response, '') AS `Response to Treatment`,
+        coalesce(co.cohort_description, '') AS `Cohort`
 </t>
   </si>
   <si>
-    <t>TC01_Canine_Filter_Breed-Akita_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC01_Canine_Filter_Breed-Akita_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN['Akita']  OPTIONAL MATCH (f:file)-[*]-&gt;(c), (samp:sample)-[*]-&gt;(c) WITH DISTINCT c AS c, p, s, demo, diag, f, samp RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(samp)) as number_of_sample , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
-  </si>
-  <si>
-    <t>StatQuery</t>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+WHERE demo.breed IN ['Akita']  
+OPTIONAL MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+WITH DISTINCT f, parent, c, demo, diag, s
+RETURN  coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_type, '') AS `File Type`,
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+        coalesce(f.file_format, '') AS `Format`,
+        coalesce(f.file_size, '') AS `Size`,
+        coalesce(c.case_id, '') AS `Case ID`,
+        coalesce(demo.breed,'') AS Breed , 
+        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+WHERE demo.breed IN ['Akita'] 
+WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(demo.breed,'') AS Breed , 
+        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
   </si>
 </sst>
 </file>
@@ -106,11 +171,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,47 +492,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="75.81640625" customWidth="1"/>
-    <col min="2" max="2" width="255.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.26953125" customWidth="1"/>
-    <col min="4" max="4" width="40.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.453125" customWidth="1"/>
+    <col min="3" max="3" width="86.1796875" customWidth="1"/>
+    <col min="4" max="4" width="70.26953125" customWidth="1"/>
+    <col min="5" max="5" width="40.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C13" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
updated a sample ICDC test script and Bento test scripts
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
+++ b/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD925796-E5D1-4A5C-B8F7-D543CBC40804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C898FAC6-B090-4250-9AFC-47F86C1614FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -88,25 +88,6 @@
 </t>
   </si>
   <si>
-    <t>MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
-WHERE demo.breed IN ['Akita']  
-OPTIONAL MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-WITH DISTINCT f, parent, c, demo, diag, s
-RETURN  coalesce(f.file_name, '') AS `File Name`,
-        coalesce(f.file_type, '') AS `File Type`,
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`,
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
 WHERE demo.breed IN ['Akita'] 
 WITH DISTINCT samp AS samp, c, demo, diag
@@ -122,6 +103,23 @@
         coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
         coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
         coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+WHERE demo.breed IN ['Akita']  
+OPTIONAL MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+WITH DISTINCT f, parent, c, demo, diag, s
+RETURN  coalesce(f.file_name, '') AS `File Name`,
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+        coalesce(f.file_format, '') AS `Format`,
+        coalesce(f.file_size, '') AS `Size`,
+        coalesce(c.case_id, '') AS `Case ID`,
+        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
   </si>
 </sst>
 </file>
@@ -494,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -546,7 +544,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
@@ -558,12 +556,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
corrected ICDC Breed 1-14 scripts
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
+++ b/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C898FAC6-B090-4250-9AFC-47F86C1614FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507F405D-C945-4AC1-8855-11C5B3C31903}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -67,44 +67,6 @@
     <t>FilesTab</t>
   </si>
   <si>
-    <t xml:space="preserve">MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-WHERE demo.breed IN ['Akita']
-MATCH (c)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co
-RETURN  coalesce(c.case_id, '') AS `Case ID` ,
-        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
-        coalesce(s.clinical_study_type, '') AS  `Study Type`,
-        coalesce(demo.breed, '') AS Breed ,
-        coalesce(diag.disease_term, '') AS Diagnosis ,
-        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
-        coalesce(demo.patient_age_at_enrollment, '') AS Age ,
-        coalesce(demo.sex, '') AS Sex ,
-        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-        coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`,
-        coalesce(co.cohort_description, '') AS `Cohort`
-</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
-WHERE demo.breed IN ['Akita'] 
-WITH DISTINCT samp AS samp, c, demo, diag
-RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(samp.sample_site, '') AS `Sample Site`,
-        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
-        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
-        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
-        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
-        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
-        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
-        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
-  </si>
-  <si>
     <t>MATCH (f:file)--&gt;(parent)
 WITH DISTINCT f, parent
 MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
@@ -120,6 +82,44 @@
         coalesce(c.case_id, '') AS `Case ID`,
         coalesce(diag.disease_term,'') AS Diagnosis , 
         coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+WHERE demo.breed IN ['Akita'] 
+WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(demo.breed,'') AS Breed,
+        coalesce(diag.disease_term,'') AS Diagnosis, 
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE demo.breed IN ['Akita']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co
+RETURN  coalesce(c.case_id, '') AS `Case ID`,
+        coalesce(s.clinical_study_designation, '') AS `Study Code`,
+        coalesce(s.clinical_study_type, '') AS  `Study Type`,
+        coalesce(demo.breed, '') AS Breed ,
+        coalesce(diag.disease_term, '') AS Diagnosis ,
+        coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
+        coalesce(demo.patient_age_at_enrollment, '') AS Age,
+        coalesce(demo.sex, '') AS Sex,
+        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+        coalesce(demo.weight, '') AS `Weight (kg)`,
+        coalesce(diag.best_response, '') AS `Response to Treatment`,
+        coalesce(co.cohort_description, '') AS `Cohort`
+</t>
   </si>
 </sst>
 </file>
@@ -492,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -527,7 +527,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -561,7 +561,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
changed the xlfile akita 01 and created regression suite laxmi_regression1
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
+++ b/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation_master\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89183A71-C894-449B-9DB0-7699214AB87B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB91598-1BBC-406A-8636-51F125F30631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -84,27 +84,6 @@
         coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
   </si>
   <si>
-    <t xml:space="preserve">MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-WHERE demo.breed IN ['Akita']
-MATCH (c)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co
-RETURN  coalesce(c.case_id, '') AS `Case ID`,
-        coalesce(s.clinical_study_designation, '') AS `Study Code`,
-        coalesce(s.clinical_study_type, '') AS  `Study Type`,
-        coalesce(demo.breed, '') AS Breed ,
-        coalesce(diag.disease_term, '') AS Diagnosis ,
-        coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
-        coalesce(demo.patient_age_at_enrollment, '') AS Age,
-        coalesce(demo.sex, '') AS Sex,
-        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-        coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`,
-        coalesce(co.cohort_description, '') AS `Cohort`
-</t>
-  </si>
-  <si>
     <t>MATCH (f:file)--&gt;(parent)
 WITH DISTINCT f, parent
 MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
@@ -122,6 +101,26 @@
         coalesce(demo.breed,'') AS Breed , 
         coalesce(diag.disease_term,'') AS Diagnosis , 
         coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE demo.breed IN ['Akita']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co
+RETURN  coalesce(c.case_id, '') AS `Case ID`,
+        coalesce(s.clinical_study_designation, '') AS `Study Code`,
+        coalesce(s.clinical_study_type, '') AS  `Study Type`,
+        coalesce(demo.breed, '') AS Breed ,
+        coalesce(diag.disease_term, '') AS Diagnosis ,
+        coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
+        coalesce(demo.patient_age_at_enrollment, '') AS Age,
+        coalesce(demo.sex, '') AS Sex,
+        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+        coalesce(demo.weight, '') AS `Weight (kg)`,
+        coalesce(diag.best_response, '') AS `Response to Treatment`
+</t>
   </si>
 </sst>
 </file>
@@ -494,20 +493,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="92.453125" customWidth="1"/>
-    <col min="3" max="3" width="86.1796875" customWidth="1"/>
-    <col min="4" max="4" width="70.26953125" customWidth="1"/>
-    <col min="5" max="5" width="40.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.42578125" customWidth="1"/>
+    <col min="3" max="3" width="86.140625" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -524,12 +523,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="270" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -541,7 +540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -558,12 +557,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -575,31 +574,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
     </row>
   </sheetData>
@@ -615,7 +614,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed StudyComb for Faceted Filters ICDC
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
+++ b/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation_master\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB91598-1BBC-406A-8636-51F125F30631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA843F02-3FCA-45F7-BEA5-E16190E94A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="37065" yWindow="1920" windowWidth="16455" windowHeight="10770" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -49,9 +49,6 @@
     <t>TC01_Canine_Filter_Breed-Akita_WebData.xlsx</t>
   </si>
   <si>
-    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN['Akita']  OPTIONAL MATCH (f:file)-[*]-&gt;(c), (samp:sample)-[*]-&gt;(c) WITH DISTINCT c AS c, p, s, demo, diag, f, samp RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(samp)) as number_of_sample , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
-  </si>
-  <si>
     <t>StatQuery</t>
   </si>
   <si>
@@ -121,6 +118,18 @@
         coalesce(demo.weight, '') AS `Weight (kg)`,
         coalesce(diag.best_response, '') AS `Response to Treatment`
 </t>
+  </si>
+  <si>
+    <t>MATCH (demo:demographic)
+WHERE demo.breed IN ["Akita"]
+MATCH (demo:demographic)--&gt;(c:case)--&gt;(s:study)--&gt;(p:program)
+OPTIONAL MATCH (c)&lt;-[*]-(samp:sample)
+OPTIONAL MATCH (c)&lt;-[*]-(f:file)
+RETURN 
+	count(DISTINCT(f)) as number_of_files, 
+	count(DISTINCT(samp)) as number_of_sample, 
+	count(DISTINCT(c)) as number_of_cases, 
+	count(DISTINCT(s)) as number_of_study</t>
   </si>
 </sst>
 </file>
@@ -493,28 +502,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="92.42578125" customWidth="1"/>
-    <col min="3" max="3" width="86.140625" customWidth="1"/>
-    <col min="4" max="4" width="70.28515625" customWidth="1"/>
-    <col min="5" max="5" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.44140625" customWidth="1"/>
+    <col min="3" max="3" width="86.109375" customWidth="1"/>
+    <col min="4" max="4" width="70.33203125" customWidth="1"/>
+    <col min="5" max="5" width="40.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -523,15 +532,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -540,15 +549,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -557,15 +566,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="255" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -574,31 +583,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
     </row>
   </sheetData>
@@ -614,7 +623,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
queries & other updates
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
+++ b/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation_master\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB91598-1BBC-406A-8636-51F125F30631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18895CD-6616-4243-A412-AF05F6F777ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>WebExcel</t>
   </si>
@@ -103,11 +103,14 @@
         coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
   </si>
   <si>
-    <t xml:space="preserve">MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+    <t xml:space="preserve">MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN['Akita']  OPTIONAL MATCH (f:file)-[*]-&gt;(c), (samp:sample)-[*]-&gt;(c) WITH DISTINCT c AS c, p, s, demo, diag, f, samp RETURN  count(DISTINCT(s.clinical_study_designation)) as Studies, count(DISTINCT(c.case_id)) as Cases ,count(DISTINCT(samp)) as Samples ,count(DISTINCT(f)) as `Case Files` </t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
 WHERE demo.breed IN ['Akita']
 MATCH (c)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+ MATCH (co:cohort)&lt;-[*]-(c)
+ OPTIONAL MATCH (samp:sample)--&gt;(c)
 WITH DISTINCT c, s, demo, diag, co
 RETURN  coalesce(c.case_id, '') AS `Case ID`,
         coalesce(s.clinical_study_designation, '') AS `Study Code`,
@@ -119,8 +122,8 @@
         coalesce(demo.sex, '') AS Sex,
         coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
         coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`
-</t>
+        coalesce(diag.best_response, '') AS `Response to Treatment`,
+        coalesce(co.cohort_description, '') AS `Cohort`</t>
   </si>
 </sst>
 </file>
@@ -494,7 +497,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,10 +531,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Fixed ICDC breed all testcases
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
+++ b/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA843F02-3FCA-45F7-BEA5-E16190E94A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05691F3B-8FA5-4AA8-B1CD-2B1B1AC46F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37065" yWindow="1920" windowWidth="16455" windowHeight="10770" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -120,16 +120,19 @@
 </t>
   </si>
   <si>
-    <t>MATCH (demo:demographic)
+    <t>MATCH (demo:demographic)--&gt;(c:case)--&gt;(s:study)--&gt;(p:program)
 WHERE demo.breed IN ["Akita"]
-MATCH (demo:demographic)--&gt;(c:case)--&gt;(s:study)--&gt;(p:program)
 OPTIONAL MATCH (c)&lt;-[*]-(samp:sample)
 OPTIONAL MATCH (c)&lt;-[*]-(f:file)
-RETURN 
-	count(DISTINCT(f)) as number_of_files, 
-	count(DISTINCT(samp)) as number_of_sample, 
-	count(DISTINCT(c)) as number_of_cases, 
-	count(DISTINCT(s)) as number_of_study</t>
+OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+  RETURN 
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
   </si>
 </sst>
 </file>
@@ -502,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated comparator; addeed study files tab to akita breed tc
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
+++ b/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Desktop\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05691F3B-8FA5-4AA8-B1CD-2B1B1AC46F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61477FA6-F595-4640-B747-EAD9BB5596AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>WebExcel</t>
   </si>
@@ -81,58 +81,96 @@
         coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
   </si>
   <si>
-    <t>MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
-WHERE demo.breed IN ['Akita']  
-OPTIONAL MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
 OPTIONAL MATCH (samp:sample)--&gt;(c)
-WITH DISTINCT f, parent, c, demo, diag, s
-RETURN coalesce(f.file_name, '') AS `File Name`, 
-        coalesce(f.file_type, '') AS `File Type`, 
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `File Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-WHERE demo.breed IN ['Akita']
-MATCH (c)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co
-RETURN  coalesce(c.case_id, '') AS `Case ID`,
-        coalesce(s.clinical_study_designation, '') AS `Study Code`,
-        coalesce(s.clinical_study_type, '') AS  `Study Type`,
-        coalesce(demo.breed, '') AS Breed ,
-        coalesce(diag.disease_term, '') AS Diagnosis ,
-        coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
-        coalesce(demo.patient_age_at_enrollment, '') AS Age,
-        coalesce(demo.sex, '') AS Sex,
-        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-        coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`
-</t>
-  </si>
-  <si>
-    <t>MATCH (demo:demographic)--&gt;(c:case)--&gt;(s:study)--&gt;(p:program)
-WHERE demo.breed IN ["Akita"]
-OPTIONAL MATCH (c)&lt;-[*]-(samp:sample)
-OPTIONAL MATCH (c)&lt;-[*]-(f:file)
+OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
 OPTIONAL MATCH (f:file)-[*]-&gt;(c)
 OPTIONAL MATCH (sf:file)--&gt;(s)
-  RETURN 
+WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
+WHERE demo.breed IN ['Akita']
+RETURN  
     count(distinct p) AS Programs,
     count(distinct s) AS Studies,
     count(distinct c) AS Cases,
     count(distinct samp) AS Samples,
     count(distinct f) AS `Case Files`,
     count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE demo.breed IN ['Akita']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age
+RETURN  
+       coalesce(c.case_id, '') AS `Case ID`,
+       coalesce(s.clinical_study_designation, '') AS `Study Code`,
+       coalesce(s.clinical_study_type, '') AS  `Study Type`,
+       coalesce(demo.breed, '') AS Breed ,
+       coalesce(diag.disease_term, '') AS Diagnosis ,
+       coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
+       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS Age,
+       coalesce(demo.sex, '') AS Sex,
+       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+       coalesce(demo.weight, '') AS `Weight (kg)`,
+       coalesce(diag.best_response, '') AS `Response to Treatment`,
+       coalesce(co.cohort_description, '') AS `Cohort`</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
+ MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+WHERE demo.breed IN ['Akita']
+OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp)
+WITH
+        f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH    
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value, 10^precision AS factor,
+        units[i] as unit
+RETURN coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_type, '') AS `File Type`,
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+        coalesce(f.file_format, '') AS `Format`,
+        round(factor * value)/factor+' ' +unit AS Size,
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(c.case_id, '') AS `Case ID`,
+        coalesce(demo.breed,'') AS Breed ,
+        coalesce(diag.disease_term,'') AS Diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  MATCH (f:file)--&gt;(s:study)
+ MATCH (f)--&gt;(parent)
+MATCH (s)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
+WHERE demo.breed  IN ['Akita']  
+WITH DISTINCT f, parent, s, c, demo, diag
+WITH
+        f, c, demo, diag, s,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH    
+        f, c, demo, diag, s,
+        f.file_size /(1024^i) AS value, 10^precision AS factor,
+        units[i] as unit
+RETURN 
+  coalesce(f.file_name, '') AS `File Name`,
+  coalesce(f.file_type, '') AS `File Type`,
+  coalesce("study", '') AS `Association`,
+  coalesce(f.file_description, '') AS `Description`,
+  coalesce(f.file_format, '') AS  Format,
+  round(factor * value)/factor+' ' +unit AS Size,
+  coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+  </si>
+  <si>
+    <t>StudyFilesTab</t>
   </si>
 </sst>
 </file>
@@ -503,22 +541,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="92.44140625" customWidth="1"/>
-    <col min="3" max="3" width="86.109375" customWidth="1"/>
-    <col min="4" max="4" width="70.33203125" customWidth="1"/>
-    <col min="5" max="5" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.42578125" customWidth="1"/>
+    <col min="3" max="3" width="86.140625" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -535,7 +573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="285" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -543,7 +581,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -552,7 +590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -560,7 +598,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -569,15 +607,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -586,32 +624,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C13" s="1"/>
+    <row r="5" spans="1:5" ht="213" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -626,7 +654,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
corrected tc1,2,46 and added study files query + comparelists
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
+++ b/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61477FA6-F595-4640-B747-EAD9BB5596AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2287B1-57E7-4527-B7E7-1FE3F182532A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -118,28 +118,36 @@
        coalesce(co.cohort_description, '') AS `Cohort`</t>
   </si>
   <si>
+    <t>StudyFilesTab</t>
+  </si>
+  <si>
     <t>MATCH (f:file)--&gt;(parent)
 WITH DISTINCT f, parent
 MATCH (diag:diagnosis)--&gt;(c)
 OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
- MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
-WHERE demo.breed IN ['Akita']
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+WHERE demo.breed IN ['Akita'] 
 OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp)
 WITH
         f, parent, c, demo, diag, s, samp,
         ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
         toInteger(floor(log(f.file_size)/log(1024))) as i,
         2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value, 
+        10^precision AS factor,
+        units[i] as unit
 WITH    
-        f, parent, c, demo, diag, s, samp,
-        f.file_size /(1024^i) AS value, 10^precision AS factor,
-        units[i] as unit
-RETURN coalesce(f.file_name, '') AS `File Name`,
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN 
+        coalesce(f.file_name, '') AS `File Name`,
         coalesce(f.file_type, '') AS `File Type`,
         coalesce(labels(parent)[0], '') AS `Association`,
         coalesce(f.file_description, '') AS `Description`,
         coalesce(f.file_format, '') AS `Format`,
-        round(factor * value)/factor+' ' +unit AS Size,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
         coalesce(samp.sample_id, '') AS `Sample ID`,
         coalesce(c.case_id, '') AS `Case ID`,
         coalesce(demo.breed,'') AS Breed ,
@@ -147,10 +155,9 @@
   </si>
   <si>
     <t xml:space="preserve">  MATCH (f:file)--&gt;(s:study)
- MATCH (f)--&gt;(parent)
 MATCH (s)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
-WHERE demo.breed  IN ['Akita']  
-WITH DISTINCT f, parent, s, c, demo, diag
+WHERE demo.breed  IN ['Akita'] 
+WITH DISTINCT f,  s, c, demo, diag
 WITH
         f, c, demo, diag, s,
         ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
@@ -160,17 +167,17 @@
         f, c, demo, diag, s,
         f.file_size /(1024^i) AS value, 10^precision AS factor,
         units[i] as unit
-RETURN 
+        WITH    
+        f,  c, demo, diag, s, unit,
+        round(factor * value)/factor AS size
+RETURN DISTINCT
   coalesce(f.file_name, '') AS `File Name`,
   coalesce(f.file_type, '') AS `File Type`,
   coalesce("study", '') AS `Association`,
   coalesce(f.file_description, '') AS `Description`,
   coalesce(f.file_format, '') AS  Format,
-  round(factor * value)/factor+' ' +unit AS Size,
+  CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
   coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
-    <t>StudyFilesTab</t>
   </si>
 </sst>
 </file>
@@ -543,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +619,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -626,10 +633,10 @@
     </row>
     <row r="5" spans="1:5" ht="213" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
curated icdc 1-8, 29, 30, 31
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
+++ b/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2287B1-57E7-4527-B7E7-1FE3F182532A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1A7812-6902-4334-80BC-83C6177D62C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -550,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
1 to 8 29-35 in ICDC
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
+++ b/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1A7812-6902-4334-80BC-83C6177D62C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37B0916-F20D-4C7A-B4DC-D5743870E776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -95,27 +95,6 @@
     count(distinct samp) AS Samples,
     count(distinct f) AS `Case Files`,
     count(distinct sf) AS `Study Files`</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-WHERE demo.breed IN ['Akita']
-MATCH (c)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age
-RETURN  
-       coalesce(c.case_id, '') AS `Case ID`,
-       coalesce(s.clinical_study_designation, '') AS `Study Code`,
-       coalesce(s.clinical_study_type, '') AS  `Study Type`,
-       coalesce(demo.breed, '') AS Breed ,
-       coalesce(diag.disease_term, '') AS Diagnosis ,
-       coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
-       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS Age,
-       coalesce(demo.sex, '') AS Sex,
-       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-       coalesce(demo.weight, '') AS `Weight (kg)`,
-       coalesce(diag.best_response, '') AS `Response to Treatment`,
-       coalesce(co.cohort_description, '') AS `Cohort`</t>
   </si>
   <si>
     <t>StudyFilesTab</t>
@@ -178,6 +157,27 @@
   coalesce(f.file_format, '') AS  Format,
   CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
   coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE demo.breed IN ['Akita']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age
+RETURN  
+       coalesce(c.case_id, '') AS `Case ID`,
+       coalesce(s.clinical_study_designation, '') AS `Study Code`,
+       coalesce(s.clinical_study_type, '') AS  `Study Type`,
+       coalesce(demo.breed, '') AS Breed ,
+       coalesce(diag.disease_term, '') AS Diagnosis ,
+       coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
+       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS Age,
+       coalesce(demo.sex, '') AS Sex,
+       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+       coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
+       coalesce(diag.best_response, '') AS `Response to Treatment`,
+       coalesce(co.cohort_description, '') AS `Cohort`</t>
   </si>
 </sst>
 </file>
@@ -551,7 +551,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,12 +580,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="285" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="300" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
@@ -619,7 +619,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -633,10 +633,10 @@
     </row>
     <row r="5" spans="1:5" ht="213" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
with neo4j fix and INS
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
+++ b/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37B0916-F20D-4C7A-B4DC-D5743870E776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99065183-1AAE-4048-B0E8-CB0CAA4ABF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -164,7 +164,7 @@
 MATCH (c)&lt;--(diag:diagnosis)
 OPTIONAL MATCH (samp:sample)--&gt;(c)
 OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
 RETURN  
        coalesce(c.case_id, '') AS `Case ID`,
        coalesce(s.clinical_study_designation, '') AS `Study Code`,
@@ -551,7 +551,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="300" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="315" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Fix all ICDC breed testcases
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
+++ b/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99065183-1AAE-4048-B0E8-CB0CAA4ABF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642A1317-5EA8-46BE-9C49-EE8961120245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="16354" yWindow="-4860" windowWidth="33120" windowHeight="18120" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -64,6 +64,25 @@
     <t>FilesTab</t>
   </si>
   <si>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
+WHERE demo.breed IN ['Akita']
+RETURN  
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>StudyFilesTab</t>
+  </si>
+  <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
 WHERE demo.breed IN ['Akita'] 
 WITH DISTINCT samp AS samp, c, demo, diag
@@ -78,59 +97,30 @@
         coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
         coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
         coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
-        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
-  </si>
-  <si>
-    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`
+Order by samp.sample_id LIMIT 100</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE demo.breed IN ['Akita']
+MATCH (c)&lt;--(diag:diagnosis)
 OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
-OPTIONAL MATCH (f:file)-[*]-&gt;(c)
-OPTIONAL MATCH (sf:file)--&gt;(s)
-WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
-WHERE demo.breed IN ['Akita']
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
 RETURN  
-    count(distinct p) AS Programs,
-    count(distinct s) AS Studies,
-    count(distinct c) AS Cases,
-    count(distinct samp) AS Samples,
-    count(distinct f) AS `Case Files`,
-    count(distinct sf) AS `Study Files`</t>
-  </si>
-  <si>
-    <t>StudyFilesTab</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (diag:diagnosis)--&gt;(c)
-OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
-WHERE demo.breed IN ['Akita'] 
-OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp)
-WITH
-        f, parent, c, demo, diag, s, samp,
-        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
-        toInteger(floor(log(f.file_size)/log(1024))) as i,
-        2 as precision
-WITH
-        f, parent, c, demo, diag, s, samp,
-        f.file_size /(1024^i) AS value, 
-        10^precision AS factor,
-        units[i] as unit
-WITH    
-        f, parent, c, demo, diag, s, samp, unit,
-        round(factor * value)/factor AS size
-RETURN 
-        coalesce(f.file_name, '') AS `File Name`,
-        coalesce(f.file_type, '') AS `File Type`,
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `Format`,
-        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
-        coalesce(samp.sample_id, '') AS `Sample ID`,
-        coalesce(c.case_id, '') AS `Case ID`,
-        coalesce(demo.breed,'') AS Breed ,
-        coalesce(diag.disease_term,'') AS Diagnosis</t>
+       coalesce(c.case_id, '') AS `Case ID`,
+       coalesce(s.clinical_study_designation, '') AS `Study Code`,
+       coalesce(s.clinical_study_type, '') AS  `Study Type`,
+       coalesce(demo.breed, '') AS Breed ,
+       coalesce(diag.disease_term, '') AS Diagnosis ,
+       coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
+       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS Age,
+       coalesce(demo.sex, '') AS Sex,
+       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+       coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
+       coalesce(diag.best_response, '') AS `Response to Treatment`,
+       coalesce(co.cohort_description, '') AS `Cohort`
+Order by c.case_id LIMIT 100</t>
   </si>
   <si>
     <t xml:space="preserve">  MATCH (f:file)--&gt;(s:study)
@@ -156,28 +146,42 @@
   coalesce(f.file_description, '') AS `Description`,
   coalesce(f.file_format, '') AS  Format,
   CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
-  coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-WHERE demo.breed IN ['Akita']
-MATCH (c)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
-RETURN  
-       coalesce(c.case_id, '') AS `Case ID`,
-       coalesce(s.clinical_study_designation, '') AS `Study Code`,
-       coalesce(s.clinical_study_type, '') AS  `Study Type`,
-       coalesce(demo.breed, '') AS Breed ,
-       coalesce(diag.disease_term, '') AS Diagnosis ,
-       coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
-       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS Age,
-       coalesce(demo.sex, '') AS Sex,
-       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-       coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
-       coalesce(diag.best_response, '') AS `Response to Treatment`,
-       coalesce(co.cohort_description, '') AS `Cohort`</t>
+  coalesce(s.clinical_study_designation,'') AS `Study Code`
+Order By f.file_name LIMIT 100</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+WHERE demo.breed IN ['Akita'] 
+OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp)
+WITH
+        f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value, 
+        10^precision AS factor,
+        units[i] as unit
+WITH    
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN 
+        coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_format, '') AS `Format`,
+        coalesce(f.file_type, '') AS `File Type`,
+       CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(c.case_id, '') AS `Case ID`,
+        coalesce(demo.breed,'') AS Breed ,
+        coalesce(diag.disease_term,'') AS Diagnosis
+Order By f.file_name LIMIT 100</t>
   </si>
 </sst>
 </file>
@@ -550,20 +554,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="92.42578125" customWidth="1"/>
-    <col min="3" max="3" width="86.140625" customWidth="1"/>
-    <col min="4" max="4" width="70.28515625" customWidth="1"/>
-    <col min="5" max="5" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.44140625" customWidth="1"/>
+    <col min="3" max="3" width="86.109375" customWidth="1"/>
+    <col min="4" max="4" width="70.33203125" customWidth="1"/>
+    <col min="5" max="5" width="40.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -580,15 +584,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="315" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -597,15 +601,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -614,15 +618,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -631,15 +635,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="213" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="213" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
@@ -661,7 +665,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Excluded failed test from ICDCRegression suite
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
+++ b/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642A1317-5EA8-46BE-9C49-EE8961120245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CF77F2-C42C-4E4C-BA43-D5E98801AF6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16354" yWindow="-4860" windowWidth="33120" windowHeight="18120" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -555,7 +555,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>